<commit_message>
Added identity schema for handle support in idrepo
Signed-off-by: dhanendra06 <dhanendra.tech@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lapBkp\projects\mosip\test9\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29E2265-608B-4658-8749-A4F3BA9818E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BA4B76-9414-4400-A6DF-2AD757BA8628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>lang_code</t>
   </si>
@@ -522,6 +522,240 @@
 			}
 		}
 	}
+}</t>
+  </si>
+  <si>
+    <t>Mosip Sample identity for handle</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>Mosip Identity for handle</t>
+  </si>
+  <si>
+    <t>{
+    "$schema": "http://json-schema.org/draft-07/schema#",
+    "description": "Identity schema for sign up",
+    "additionalProperties": false,
+    "title": "signup identity",
+    "type": "object",
+    "definitions": {
+         "simpleType": {
+      "uniqueItems": true,
+      "additionalItems": false,
+      "type": "array",
+      "items": {
+        "additionalProperties": false,
+        "type": "object",
+        "required": [
+          "language",
+          "value"
+        ],
+        "properties": {
+          "language": {
+            "type": "string"
+          },
+          "value": {
+            "type": "string"
+          }
+        }
+      }
+    },
+        "TaggedListType": {
+            "uniqueItems": true,
+            "additionalItems": false,
+            "type": "array",
+            "items": {
+                "additionalProperties": false,
+                "type": "object",
+                "required": [
+                    "value"
+                ],
+                "properties": {
+                    "value": {
+                        "type": "string"
+                    },
+                    "tags": {
+                        "uniqueItems": true,
+                        "type": "array",
+                        "items": {
+                            "type": "string",
+                            "enum": [
+                                "notification",
+                                "handle"
+                            ]
+                        }
+                    }
+                }
+            }
+        },
+        "documentType": {
+            "additionalProperties": false,
+            "type": "object",
+            "properties": {
+                "format": {
+                    "type": "string"
+                },
+                "type": {
+                    "type": "string"
+                },
+                "value": {
+                    "type": "string"
+                }
+            }
+        },
+        "biometricsType": {
+            "additionalProperties": false,
+            "type": "object",
+            "properties": {
+                "format": {
+                    "type": "string"
+                },
+                "version": {
+                    "type": "number",
+                    "minimum": 0
+                },
+                "value": {
+                    "type": "string"
+                }
+            }
+        },
+        "hashType": {
+            "additionalProperties": false,
+            "type": "object",
+            "properties": {
+                "hash": {
+                    "type": "string"
+                },
+                "salt": {
+                    "type": "string"
+                }
+            }
+        }
+    },
+    "properties": {
+        "identity": {
+            "additionalProperties": false,
+            "type": "object",
+            "required": [
+                "IDSchemaVersion",
+                "fullName",
+                "phone",
+                "password",
+                "preferredLang"
+            ],
+            "properties": {
+                "UIN": {
+                    "bioAttributes": [],
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "IDSchemaVersion": {
+                    "bioAttributes": [],
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "number",
+                    "fieldType": "default",
+                    "minimum": 0
+                },
+                "selectedHandles": {
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "array",
+                    "items": {
+                        "type": "string"
+                    },
+                    "fieldType": "default"
+                },
+                "fullName": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).",
+                            "arguments": [],
+                            "type": "regex"
+                        },
+                        {
+                            "validator": "^[\u1780-\u17FF\u19E0-\u19FF\u1A00-\u1A9F\u0020]{1,30}$",
+                            "arguments": [],
+                            "type": "regex",
+                            "langCode": "khm"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/simpleType"
+                },
+                "phone": {
+                    "bioAttributes": [],
+                    "validators": [],
+                    "$ref": "#/definitions/TaggedListType",
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default",
+                    "requiredOn": "",
+                    "handle": true
+                },
+                "password": {
+                    "bioAttributes": [],
+                    "validators": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#/definitions/hashType"
+                },
+                "preferredLang": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "(^eng$|^khm$)",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "type": "string"
+                },
+                "registrationType": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^L[1-2]{1}$",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "type": "string"
+                },
+                "phoneVerified": {
+                    "bioAttributes": [],
+                    "validators": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "type": "boolean"
+                },
+                "updatedAt": {
+                    "bioAttributes": [],
+                    "validators": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "type": "number"
+                }
+            }
+        }
+    }
 }</t>
   </si>
 </sst>
@@ -910,18 +1144,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ2"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.453125" style="1"/>
-    <col min="2" max="2" width="8.453125" style="2"/>
+    <col min="2" max="2" width="8.453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="53.7265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.7265625" style="1" customWidth="1"/>
@@ -996,6 +1230,38 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:10" ht="186" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
updated identity schema for handle
Signed-off-by: dhanendra06 <dhanendra.tech@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lapBkp\projects\mosip\test9\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BA4B76-9414-4400-A6DF-2AD757BA8628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7659E8-FF37-4838-9271-1C8E891E1F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,34 +535,34 @@
   </si>
   <si>
     <t>{
-    "$schema": "http://json-schema.org/draft-07/schema#",
-    "description": "Identity schema for sign up",
+    "$schema": "http:\/\/json-schema.org\/draft-07\/schema#",
+    "description": "MOSIP Sample identity",
     "additionalProperties": false,
-    "title": "signup identity",
+    "title": "MOSIP identity",
     "type": "object",
     "definitions": {
-         "simpleType": {
-      "uniqueItems": true,
-      "additionalItems": false,
-      "type": "array",
-      "items": {
-        "additionalProperties": false,
-        "type": "object",
-        "required": [
-          "language",
-          "value"
-        ],
-        "properties": {
-          "language": {
-            "type": "string"
-          },
-          "value": {
-            "type": "string"
-          }
-        }
-      }
-    },
-        "TaggedListType": {
+        "simpleType": {
+            "uniqueItems": true,
+            "additionalItems": false,
+            "type": "array",
+            "items": {
+                "additionalProperties": false,
+                "type": "object",
+                "required": [
+                    "language",
+                    "value"
+                ],
+                "properties": {
+                    "language": {
+                        "type": "string"
+                    },
+                    "value": {
+                        "type": "string"
+                    }
+                }
+            }
+        },
+   "taggedListType": {
             "uniqueItems": true,
             "additionalItems": false,
             "type": "array",
@@ -602,6 +602,12 @@
                 },
                 "value": {
                     "type": "string"
+                },
+                "refNumber": {
+                    "type": [
+                        "string",
+                        "null"
+                    ]
                 }
             }
         },
@@ -617,18 +623,6 @@
                     "minimum": 0
                 },
                 "value": {
-                    "type": "string"
-                }
-            }
-        },
-        "hashType": {
-            "additionalProperties": false,
-            "type": "object",
-            "properties": {
-                "hash": {
-                    "type": "string"
-                },
-                "salt": {
                     "type": "string"
                 }
             }
@@ -641,79 +635,41 @@
             "required": [
                 "IDSchemaVersion",
                 "fullName",
+                "dateOfBirth",
+                "gender",
+                "addressLine1",
+                "addressLine2",
+                "addressLine3",
+                "region",
+                "province",
+                "city",
+                "zone",
+                "postalCode",
                 "phone",
-                "password",
-                "preferredLang"
+                "email",
+                "proofOfIdentity",
+                "individualBiometrics"
             ],
             "properties": {
-                "UIN": {
-                    "bioAttributes": [],
-                    "fieldCategory": "none",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default"
-                },
-                "IDSchemaVersion": {
-                    "bioAttributes": [],
-                    "fieldCategory": "none",
-                    "format": "none",
-                    "type": "number",
-                    "fieldType": "default",
-                    "minimum": 0
-                },
-                "selectedHandles": {
-                    "fieldCategory": "none",
-                    "format": "none",
-                    "type": "array",
-                    "items": {
-                        "type": "string"
-                    },
-                    "fieldType": "default"
-                },
-                "fullName": {
+                "proofOfAddress": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/documentType"
+                },
+                "gender": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "city": {
                     "bioAttributes": [],
                     "validators": [
                         {
-                            "validator": "^(?=.{3,50}$).",
-                            "arguments": [],
-                            "type": "regex"
-                        },
-                        {
-                            "validator": "^[\u1780-\u17FF\u19E0-\u19FF\u1A00-\u1A9F\u0020]{1,30}$",
-                            "arguments": [],
-                            "type": "regex",
-                            "langCode": "khm"
-                        }
-                    ],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#/definitions/simpleType"
-                },
-                "phone": {
-                    "bioAttributes": [],
-                    "validators": [],
-                    "$ref": "#/definitions/TaggedListType",
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "type": "string",
-                    "fieldType": "default",
-                    "requiredOn": "",
-                    "handle": true
-                },
-                "password": {
-                    "bioAttributes": [],
-                    "validators": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "$ref": "#/definitions/hashType"
-                },
-                "preferredLang": {
-                    "bioAttributes": [],
-                    "validators": [
-                        {
-                            "validator": "(^eng$|^khm$)",
+                            "validator": "^(?=.{0,50}$).*",
                             "arguments": [],
                             "type": "regex"
                         }
@@ -721,37 +677,316 @@
                     "fieldCategory": "pvt",
                     "format": "none",
                     "fieldType": "default",
-                    "type": "string"
-                },
-                "registrationType": {
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "postalCode": {
                     "bioAttributes": [],
                     "validators": [
                         {
-                            "validator": "^L[1-2]{1}$",
+                            "validator": "^[(?i)A-Z0-9]{5}$|^NA$",
                             "arguments": [],
                             "type": "regex"
                         }
                     ],
                     "fieldCategory": "pvt",
                     "format": "none",
-                    "fieldType": "default",
-                    "type": "string"
-                },
-                "phoneVerified": {
-                    "bioAttributes": [],
-                    "validators": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "type": "boolean"
-                },
-                "updatedAt": {
-                    "bioAttributes": [],
-                    "validators": [],
-                    "fieldCategory": "pvt",
-                    "format": "none",
-                    "fieldType": "default",
-                    "type": "number"
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "proofOfException-1": {
+                    "bioAttributes": [],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/documentType"
+                },
+                "referenceIdentityNumber": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^([0-9]{10,30})$",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "kyc",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "individualBiometrics": {
+                    "bioAttributes": [
+                        "leftEye",
+                        "rightEye",
+                        "rightIndex",
+                        "rightLittle",
+                        "rightRing",
+                        "rightMiddle",
+                        "leftIndex",
+                        "leftLittle",
+                        "leftRing",
+                        "leftMiddle",
+                        "leftThumb",
+                        "rightThumb",
+                        "face"
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/biometricsType"
+                },
+                "province": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "zone": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "proofOfDateOfBirth": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/documentType"
+                },
+                "addressLine1": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "addressLine2": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).*",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "residenceStatus": {
+                    "bioAttributes": [],
+                    "fieldCategory": "kyc",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "addressLine3": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).*",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "email": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "introducerRID": {
+                    "bioAttributes": [],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "introducerBiometrics": {
+                    "bioAttributes": [
+                        "leftEye",
+                        "rightEye",
+                        "rightIndex",
+                        "rightLittle",
+                        "rightRing",
+                        "rightMiddle",
+                        "leftIndex",
+                        "leftLittle",
+                        "leftRing",
+                        "leftMiddle",
+                        "leftThumb",
+                        "rightThumb",
+                        "face"
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/biometricsType"
+                },
+                "fullName": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{3,50}$).*",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "dateOfBirth": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])\/([0][1-9]|1[0-2])\/([0][1-9]|[1-2][0-9]|3[01])$",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "individualAuthBiometrics": {
+                    "bioAttributes": [
+                        "leftEye",
+                        "rightEye",
+                        "rightIndex",
+                        "rightLittle",
+                        "rightRing",
+                        "rightMiddle",
+                        "leftIndex",
+                        "leftLittle",
+                        "leftRing",
+                        "leftMiddle",
+                        "leftThumb",
+                        "rightThumb",
+                        "face"
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/biometricsType"
+                },
+                "introducerUIN": {
+                    "bioAttributes": [],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "proofOfIdentity": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/documentType"
+                },
+                "IDSchemaVersion": {
+                    "bioAttributes": [],
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "number",
+                    "fieldType": "default",
+                    "minimum": 0
+                },
+                "proofOfException": {
+                    "bioAttributes": [],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/documentType"
+                },
+                "phone": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^[+]*([0-9]{1})([0-9]{9})$",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "introducerName": {
+                    "bioAttributes": [],
+                    "fieldCategory": "evidence",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
+                },
+                "proofOfRelationship": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/documentType"
+                },
+                "UIN": {
+                    "bioAttributes": [],
+                    "fieldCategory": "none",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "default"
+                },
+                "preferredLang": {
+                    "bioAttributes": [],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "type": "string",
+                    "fieldType": "dynamic"
+                },
+                "region": {
+                    "bioAttributes": [],
+                    "validators": [
+                        {
+                            "validator": "^(?=.{0,50}$).*",
+                            "arguments": [],
+                            "type": "regex"
+                        }
+                    ],
+                    "fieldCategory": "pvt",
+                    "format": "none",
+                    "fieldType": "default",
+                    "$ref": "#\/definitions\/simpleType"
                 }
             }
         }
@@ -763,7 +998,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -776,6 +1011,12 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -813,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -829,6 +1070,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,7 +1391,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1230,7 +1474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="186" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="274.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1246,7 +1490,7 @@
       <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">

</xml_diff>

<commit_message>
Added definitions for hashType
Signed-off-by: dhanendra06 <dhanendra.tech@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/identity_schema.xlsx
+++ b/mosip_master/xlsx/identity_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lapBkp\projects\mosip\test9\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7659E8-FF37-4838-9271-1C8E891E1F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F18BC6-38BB-4908-A72E-97DEC9B32293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,7 @@
                 }
             }
         },
-   "taggedListType": {
+        "taggedListType": {
             "uniqueItems": true,
             "additionalItems": false,
             "type": "array",
@@ -587,6 +587,18 @@
                             ]
                         }
                     }
+                }
+            }
+        },
+        "hashType": {
+            "additionalProperties": false,
+            "type": "object",
+            "properties": {
+                "hash": {
+                    "type": "string"
+                },
+                "salt": {
+                    "type": "string"
                 }
             }
         },
@@ -1391,7 +1403,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>